<commit_message>
Misc. minor updates and fixes
* Made a few minor corrections to fix typos and delete unnecessary
comments/code

* Changed the default sizing for sleep graphs; automatic graphs should
now be easier to view without needing to change the boundaries

* Updated sample input file to be more illustrative of the current data
input system

* Commented out periodicity calculations in actogram2master. These lines
of code were causing the program to break; a future release will solve
this problem. I flagged the lines of code that involve periodicity
calculations, and left the old (commented out) code directly under the
code that excludes the periodicity analysis.
</commit_message>
<xml_diff>
--- a/sample input file.xlsx
+++ b/sample input file.xlsx
@@ -19,21 +19,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>Monitor120</t>
-  </si>
-  <si>
-    <t>12 Sep 14</t>
-  </si>
-  <si>
-    <t>16 Sep 14</t>
   </si>
   <si>
     <t>C'-ple</t>
   </si>
   <si>
     <t>D-GFP</t>
+  </si>
+  <si>
+    <t>16 Aug 15</t>
+  </si>
+  <si>
+    <t>12 Aug 15</t>
+  </si>
+  <si>
+    <t>1:11</t>
+  </si>
+  <si>
+    <t>12:32</t>
   </si>
 </sst>
 </file>
@@ -194,13 +200,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="103">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -610,12 +617,12 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.85546875" style="1"/>
@@ -625,12 +632,12 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -640,10 +647,10 @@
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="1">
-        <v>11</v>
+        <v>1</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>5</v>
       </c>
       <c r="D3" s="1">
         <v>1</v>
@@ -654,10 +661,10 @@
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="1">
-        <v>14</v>
+        <v>2</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>6</v>
       </c>
       <c r="D4" s="1">
         <v>1</v>

</xml_diff>